<commit_message>
removed superfluous formula tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test-valid-formula.xlsx
+++ b/src/test/resources/test-valid-formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="10995"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="9510" windowHeight="3705"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>MyInteger</t>
   </si>
   <si>
     <t>MyFormulaInteger</t>
+  </si>
+  <si>
+    <t>MyDate</t>
+  </si>
+  <si>
+    <t>MyTime</t>
+  </si>
+  <si>
+    <t>MyFormulaTimestamp</t>
   </si>
 </sst>
 </file>
@@ -57,8 +66,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -361,17 +374,28 @@
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -379,14 +403,34 @@
         <f>A2+Sheet2!A1</f>
         <v>4</v>
       </c>
+      <c r="C2" s="1">
+        <v>41147</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.56777777777777783</v>
+      </c>
+      <c r="E2" s="4">
+        <f>C2+D2</f>
+        <v>41147.567777777775</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f>Sheet2!A2-Sheet1!A3</f>
         <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>37240</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <f>C3+D3</f>
+        <v>37240.212500000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>